<commit_message>
Updated nhd September 2025
</commit_message>
<xml_diff>
--- a/caches/geolocations.xlsx
+++ b/caches/geolocations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="1282">
   <si>
     <t xml:space="preserve">209 Fisherville Road,Concord,03301</t>
   </si>
@@ -3839,6 +3839,33 @@
   </si>
   <si>
     <t>551 Pine River Pond Road,Sanbornville,03872</t>
+  </si>
+  <si>
+    <t>1600 Woodbury Ave.,Portsmouth,03801</t>
+  </si>
+  <si>
+    <t>80 Barnes Road,North Conway,03860</t>
+  </si>
+  <si>
+    <t>92 Farmington Road,Rochester,03867</t>
+  </si>
+  <si>
+    <t>49 Amoskeag Street,Manchester,03102</t>
+  </si>
+  <si>
+    <t>15 Dartmouth Drive,Auburn,03032</t>
+  </si>
+  <si>
+    <t>60 D'Amante Drive,Concord,03301</t>
+  </si>
+  <si>
+    <t>1279 Hooksett Road,Hooksett,03106</t>
+  </si>
+  <si>
+    <t>20 South Main Street,Concord,03301</t>
+  </si>
+  <si>
+    <t>563 Route 106 North Unit4,Loudon,03307</t>
   </si>
 </sst>
 </file>
@@ -18295,6 +18322,108 @@
         <v>-71.0437582</v>
       </c>
     </row>
+    <row r="1265">
+      <c r="A1265" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B1265">
+        <v>43.089011</v>
+      </c>
+      <c r="C1265">
+        <v>-70.79229819999999</v>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B1266">
+        <v>44.025896</v>
+      </c>
+      <c r="C1266">
+        <v>-71.114288</v>
+      </c>
+      <c r="D1266" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B1267">
+        <v>43.3320722</v>
+      </c>
+      <c r="C1267">
+        <v>-71.0098146</v>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B1268">
+        <v>43.0047946</v>
+      </c>
+      <c r="C1268">
+        <v>-71.4730697</v>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B1269">
+        <v>43.0110977</v>
+      </c>
+      <c r="C1269">
+        <v>-71.389059</v>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B1270">
+        <v>43.2205627</v>
+      </c>
+      <c r="C1270">
+        <v>-71.486426</v>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B1271">
+        <v>43.050158</v>
+      </c>
+      <c r="C1271">
+        <v>-71.43647560000001</v>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B1272">
+        <v>43.2034366</v>
+      </c>
+      <c r="C1272">
+        <v>-71.53579959999999</v>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B1273">
+        <v>43.3252388</v>
+      </c>
+      <c r="C1273">
+        <v>-71.4786416</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLinesSet="true"/>
   <pageMargins bottom="0.75" footer="0.511811023622047" header="0.511811023622047" left="0.7" right="0.7" top="0.75"/>

</xml_diff>